<commit_message>
modified home/存股/複利計算.xlsx at 2018/03/31
</commit_message>
<xml_diff>
--- a/home/存股/複利計算.xlsx
+++ b/home/存股/複利計算.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="8640"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -88,11 +88,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -367,18 +370,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -435,32 +438,32 @@
         <v>654539.10600000003</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" si="0">F3-A3</f>
-        <v>374261.89399999997</v>
+        <f t="shared" ref="B3:B16" si="0">F3-A3</f>
+        <v>571149.89399999997</v>
       </c>
       <c r="C3" s="1">
         <v>0.04</v>
       </c>
       <c r="D3">
         <f>(A3+B3)*C3</f>
-        <v>41152.04</v>
+        <v>49027.56</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E21" si="1">A3+B3+D3</f>
-        <v>1069953.04</v>
-      </c>
-      <c r="F3">
-        <v>1028801</v>
+        <v>1274716.56</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1225689</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="2">E3</f>
-        <v>1069953.04</v>
+        <v>1274716.56</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>430046.95999999996</v>
+        <v>225283.43999999994</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>
@@ -650,169 +653,219 @@
         <f t="shared" si="2"/>
         <v>5200000</v>
       </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
       <c r="C12" s="1">
         <v>0.04</v>
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>208000</v>
+        <v>220000</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>5408000</v>
+        <v>5720000</v>
+      </c>
+      <c r="F12">
+        <v>5500000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
         <f t="shared" si="2"/>
-        <v>5408000</v>
+        <v>5720000</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>280000</v>
       </c>
       <c r="C13" s="1">
         <v>0.04</v>
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>216320</v>
+        <v>240000</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>5624320</v>
+        <v>6240000</v>
+      </c>
+      <c r="F13">
+        <v>6000000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
         <f t="shared" si="2"/>
-        <v>5624320</v>
+        <v>6240000</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>260000</v>
       </c>
       <c r="C14" s="1">
         <v>0.04</v>
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>224972.80000000002</v>
+        <v>260000</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>5849292.7999999998</v>
+        <v>6760000</v>
+      </c>
+      <c r="F14">
+        <v>6500000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
         <f t="shared" si="2"/>
-        <v>5849292.7999999998</v>
+        <v>6760000</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>240000</v>
       </c>
       <c r="C15" s="1">
         <v>0.04</v>
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>233971.712</v>
+        <v>280000</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>6083264.5120000001</v>
+        <v>7280000</v>
+      </c>
+      <c r="F15">
+        <v>7000000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
         <f t="shared" si="2"/>
-        <v>6083264.5120000001</v>
+        <v>7280000</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>220000</v>
       </c>
       <c r="C16" s="1">
         <v>0.04</v>
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>243330.58048</v>
+        <v>300000</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>6326595.0924800001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>7800000</v>
+      </c>
+      <c r="F16">
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <f t="shared" si="2"/>
-        <v>6326595.0924800001</v>
+        <v>7800000</v>
       </c>
       <c r="C17" s="1">
         <v>0.04</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>253063.80369920001</v>
+        <v>312000</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>6579658.8961792002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>8112000</v>
+      </c>
+      <c r="F17">
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <f t="shared" si="2"/>
-        <v>6579658.8961792002</v>
+        <v>8112000</v>
       </c>
       <c r="C18" s="1">
         <v>0.04</v>
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>263186.35584716802</v>
+        <v>324480</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>6842845.2520263679</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>8436480</v>
+      </c>
+      <c r="F18">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <f t="shared" si="2"/>
-        <v>6842845.2520263679</v>
+        <v>8436480</v>
       </c>
       <c r="C19" s="1">
         <v>0.04</v>
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>273713.81008105475</v>
+        <v>337459.20000000001</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>7116559.0621074224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>8773939.1999999993</v>
+      </c>
+      <c r="F19">
+        <v>8500000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" si="2"/>
-        <v>7116559.0621074224</v>
+        <v>8773939.1999999993</v>
       </c>
       <c r="C20" s="1">
         <v>0.04</v>
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>284662.3624842969</v>
+        <v>350957.56799999997</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>7401221.4245917192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>9124896.7679999992</v>
+      </c>
+      <c r="F20">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" si="2"/>
-        <v>7401221.4245917192</v>
+        <v>9124896.7679999992</v>
       </c>
       <c r="C21" s="1">
         <v>0.04</v>
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>296048.85698366875</v>
+        <v>364995.87071999995</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>7697270.2815753883</v>
+        <v>9489892.6387199983</v>
+      </c>
+      <c r="F21">
+        <v>9500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified home/存股/複利計算.xlsx at 2018/04/09
</commit_message>
<xml_diff>
--- a/home/存股/複利計算.xlsx
+++ b/home/存股/複利計算.xlsx
@@ -370,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,7 +381,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -439,31 +439,31 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B16" si="0">F3-A3</f>
-        <v>571149.89399999997</v>
+        <v>627820.89399999997</v>
       </c>
       <c r="C3" s="1">
         <v>0.04</v>
       </c>
       <c r="D3">
         <f>(A3+B3)*C3</f>
-        <v>49027.56</v>
+        <v>51294.400000000001</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E21" si="1">A3+B3+D3</f>
-        <v>1274716.56</v>
+        <v>1333654.3999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>1225689</v>
+        <v>1282360</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="2">E3</f>
-        <v>1274716.56</v>
+        <v>1333654.3999999999</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>225283.43999999994</v>
+        <v>166345.60000000009</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>

</xml_diff>